<commit_message>
Added slides for test flight digital twin alignment.
</commit_message>
<xml_diff>
--- a/trng-data-summary.xlsx
+++ b/trng-data-summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mir\cam\alvium_undistorted\models\00\dataset\spt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekworth/Documents/AFIT/AAR Research/aar/students/derek.worth/pubs/rvmtl/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701F0AE8-D95B-4964-A4CD-28135967481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74FD822-C1DD-F741-AD68-1FB62955321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{ADE59AE5-24CB-46E0-BC19-912385FF76CC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" activeTab="5" xr2:uid="{ADE59AE5-24CB-46E0-BC19-912385FF76CC}"/>
   </bookViews>
   <sheets>
     <sheet name="cmds" sheetId="5" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
     <sheet name="remote trng" sheetId="6" r:id="rId4"/>
     <sheet name="confusion" sheetId="8" r:id="rId5"/>
-    <sheet name="summary" sheetId="1" r:id="rId6"/>
-    <sheet name="flt test" sheetId="2" r:id="rId7"/>
-    <sheet name="polygon" sheetId="3" r:id="rId8"/>
+    <sheet name="experiments" sheetId="9" r:id="rId6"/>
+    <sheet name="summary" sheetId="1" r:id="rId7"/>
+    <sheet name="flt test" sheetId="2" r:id="rId8"/>
+    <sheet name="polygon" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'flt test'!$I$15:$M$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'flt test'!$I$15:$M$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">planner!$B$24:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'remote trng'!$A$1:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">summary!$B$12:$F$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">summary!$B$12:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="184">
   <si>
     <t>x</t>
   </si>
@@ -530,13 +531,85 @@
   </si>
   <si>
     <t>exported</t>
+  </si>
+  <si>
+    <t>qualitative</t>
+  </si>
+  <si>
+    <t>quantitative</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>night</t>
+  </si>
+  <si>
+    <t>straight and level</t>
+  </si>
+  <si>
+    <t>banks</t>
+  </si>
+  <si>
+    <t>glare</t>
+  </si>
+  <si>
+    <t>features vs lighting</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t># of features</t>
+  </si>
+  <si>
+    <t>PtD error</t>
+  </si>
+  <si>
+    <t>OptiTrack truth</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>test flight</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>subcondition</t>
+  </si>
+  <si>
+    <t>metric/criteria</t>
+  </si>
+  <si>
+    <t>in/out/tf</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>realistic PtD vector</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>moving cam</t>
+  </si>
+  <si>
+    <t>MTL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,8 +660,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,8 +704,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -879,13 +970,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1060,10 +1167,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3606,15 +3718,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>447675</xdr:colOff>
+          <xdr:colOff>444500</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3656,15 +3768,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>254000</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>542925</xdr:colOff>
+          <xdr:colOff>546100</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>88900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4027,14 +4139,14 @@
       <selection activeCell="M8" sqref="M2:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="9.140625" style="13"/>
-    <col min="13" max="13" width="9.140625" style="19"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="12" width="9.1640625" style="13"/>
+    <col min="13" max="13" width="9.1640625" style="19"/>
+    <col min="14" max="16384" width="9.1640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
@@ -4075,7 +4187,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>119</v>
       </c>
@@ -4103,7 +4215,7 @@
         <v>$script_renumber aug/no-prb/images png 1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>119</v>
       </c>
@@ -4131,7 +4243,7 @@
         <v>$script_renumber aug/prb/images png 34435</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>119</v>
       </c>
@@ -4159,7 +4271,7 @@
         <v>$script_renumber lab/no-prb/images png 45188</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>119</v>
       </c>
@@ -4187,7 +4299,7 @@
         <v>$script_renumber lab/prb/images png 79622</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>119</v>
       </c>
@@ -4215,7 +4327,7 @@
         <v>$script_renumber real/images png 90375</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>119</v>
       </c>
@@ -4243,7 +4355,7 @@
         <v>$script_renumber virt/drg/images png 91364</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>119</v>
       </c>
@@ -4271,7 +4383,7 @@
         <v>$script_renumber virt/none/images png 106494</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="45"/>
@@ -4289,7 +4401,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
         <v>119</v>
       </c>
@@ -4317,7 +4429,7 @@
         <v>$script_renumber aug/no-prb/labels txt 1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="44" t="s">
         <v>119</v>
       </c>
@@ -4345,7 +4457,7 @@
         <v>$script_renumber aug/prb/labels txt 34435</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
         <v>119</v>
       </c>
@@ -4373,7 +4485,7 @@
         <v>$script_renumber lab/no-prb/labels txt 45188</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
         <v>119</v>
       </c>
@@ -4401,7 +4513,7 @@
         <v>$script_renumber lab/prb/labels txt 79622</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
         <v>119</v>
       </c>
@@ -4429,7 +4541,7 @@
         <v>$script_renumber real/labels txt 90375</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="44" t="s">
         <v>119</v>
       </c>
@@ -4457,7 +4569,7 @@
         <v>$script_renumber virt/drg/labels txt 91364</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
         <v>119</v>
       </c>
@@ -4485,7 +4597,7 @@
         <v>$script_renumber virt/none/labels txt 106494</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="45"/>
@@ -4503,7 +4615,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="45"/>
@@ -4521,7 +4633,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="45"/>
@@ -4539,7 +4651,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="45"/>
@@ -4557,7 +4669,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
@@ -4575,7 +4687,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="45"/>
@@ -4593,7 +4705,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="45"/>
@@ -4611,7 +4723,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="45"/>
@@ -4629,7 +4741,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="45"/>
@@ -4647,7 +4759,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="45"/>
@@ -4665,7 +4777,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="45"/>
@@ -4683,7 +4795,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="45"/>
@@ -4701,7 +4813,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="45"/>
@@ -4719,7 +4831,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="45"/>
@@ -4737,7 +4849,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="46"/>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -4755,7 +4867,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="45"/>
@@ -4773,7 +4885,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="44"/>
       <c r="B33" s="44"/>
       <c r="C33" s="45"/>
@@ -4791,7 +4903,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="45"/>
@@ -4809,7 +4921,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="45"/>
@@ -4827,7 +4939,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="44"/>
       <c r="B36" s="44"/>
       <c r="C36" s="45"/>
@@ -4845,7 +4957,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="44"/>
       <c r="B37" s="44"/>
       <c r="C37" s="45"/>
@@ -4863,7 +4975,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="44"/>
       <c r="B38" s="44"/>
       <c r="C38" s="45"/>
@@ -4881,7 +4993,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="44"/>
       <c r="B39" s="44"/>
       <c r="C39" s="45"/>
@@ -4899,7 +5011,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="44"/>
       <c r="B40" s="44"/>
       <c r="C40" s="45"/>
@@ -4917,7 +5029,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="46"/>
       <c r="B41" s="46"/>
       <c r="C41" s="46"/>
@@ -4935,7 +5047,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="46"/>
       <c r="B42" s="46"/>
       <c r="C42" s="46"/>
@@ -4953,7 +5065,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="46"/>
       <c r="B43" s="46"/>
       <c r="C43" s="46"/>
@@ -4971,7 +5083,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="46"/>
       <c r="B44" s="46"/>
       <c r="C44" s="46"/>
@@ -4989,7 +5101,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="46"/>
       <c r="B45" s="46"/>
       <c r="C45" s="46"/>
@@ -5007,7 +5119,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="46"/>
       <c r="B46" s="46"/>
       <c r="C46" s="46"/>
@@ -5025,7 +5137,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="46"/>
       <c r="B47" s="46"/>
       <c r="C47" s="46"/>
@@ -5043,7 +5155,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="46"/>
       <c r="B48" s="46"/>
       <c r="C48" s="46"/>
@@ -5061,7 +5173,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="46"/>
       <c r="B49" s="46"/>
       <c r="C49" s="46"/>
@@ -5079,7 +5191,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="46"/>
       <c r="B50" s="46"/>
       <c r="C50" s="46"/>
@@ -5097,7 +5209,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="46"/>
       <c r="B51" s="46"/>
       <c r="C51" s="46"/>
@@ -5115,7 +5227,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="46"/>
       <c r="B52" s="46"/>
       <c r="C52" s="46"/>
@@ -5141,24 +5253,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E949B6-C661-47E6-943B-6A28E38D5565}">
-  <dimension ref="B1:R56"/>
+  <dimension ref="B1:T56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:L7"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="13" customWidth="1"/>
-    <col min="2" max="13" width="9.140625" style="13"/>
-    <col min="14" max="14" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="2.5" style="13" customWidth="1"/>
+    <col min="2" max="13" width="9.1640625" style="13"/>
+    <col min="14" max="14" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N1" s="13"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E2" s="60" t="s">
         <v>44</v>
       </c>
@@ -5177,7 +5289,7 @@
       <c r="L2" s="61"/>
       <c r="N2" s="13"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="22" t="s">
         <v>36</v>
       </c>
@@ -5213,7 +5325,7 @@
       </c>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="21">
         <v>0</v>
       </c>
@@ -5249,7 +5361,7 @@
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="21">
         <v>0</v>
       </c>
@@ -5285,7 +5397,7 @@
       </c>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="21">
         <v>0</v>
       </c>
@@ -5321,7 +5433,7 @@
       </c>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="21">
         <v>1</v>
       </c>
@@ -5357,7 +5469,7 @@
       </c>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="21">
         <v>1</v>
       </c>
@@ -5393,7 +5505,7 @@
       </c>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="21">
         <v>1</v>
       </c>
@@ -5429,7 +5541,7 @@
       </c>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21">
         <v>1</v>
       </c>
@@ -5465,7 +5577,7 @@
       </c>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E11" s="13" t="s">
         <v>95</v>
       </c>
@@ -5492,13 +5604,13 @@
       </c>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="22" t="s">
         <v>54</v>
       </c>
@@ -5536,7 +5648,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21" t="s">
         <v>81</v>
       </c>
@@ -5582,7 +5694,7 @@
         <v>34434</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
         <v>82</v>
       </c>
@@ -5625,7 +5737,7 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="34" t="s">
         <v>83</v>
       </c>
@@ -5669,7 +5781,7 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
         <v>84</v>
       </c>
@@ -5710,7 +5822,7 @@
         <v>79621</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
         <v>85</v>
       </c>
@@ -5751,7 +5863,7 @@
         <v>90374</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C20" s="63" t="s">
         <v>94</v>
       </c>
@@ -5779,7 +5891,7 @@
         <v>90374</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M21" s="13" t="s">
         <v>81</v>
       </c>
@@ -5798,7 +5910,7 @@
         <v>91363</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M22" s="13" t="s">
         <v>84</v>
       </c>
@@ -5817,7 +5929,7 @@
         <v>106493</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M23" s="13" t="s">
         <v>82</v>
       </c>
@@ -5836,7 +5948,7 @@
         <v>107383</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>54</v>
       </c>
@@ -5847,7 +5959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
         <v>36</v>
       </c>
@@ -5858,7 +5970,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>37</v>
       </c>
@@ -5890,7 +6002,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>38</v>
       </c>
@@ -5924,7 +6036,7 @@
         <v>a=subsets/r-d/15130/probe</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>39</v>
       </c>
@@ -5959,7 +6071,7 @@
         <v>b=subsets/v-d/15130/probe</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>86</v>
       </c>
@@ -5994,7 +6106,7 @@
         <v>c=subsets/a-d/15130/probe</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>60</v>
       </c>
@@ -6029,7 +6141,7 @@
         <v>d=subsets/r-d/7565/probe</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="13" t="s">
         <v>87</v>
       </c>
@@ -6064,7 +6176,7 @@
         <v>e=subsets/v-d/7565/probe</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
         <v>40</v>
       </c>
@@ -6099,7 +6211,7 @@
         <v>f=subsets/a-d/7565/probe</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>88</v>
       </c>
@@ -6134,7 +6246,7 @@
         <v>g=subsets/r-d/5044/probe</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B34" s="51" t="s">
         <v>63</v>
       </c>
@@ -6175,7 +6287,7 @@
         <v>85010</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B35" s="51" t="s">
         <v>64</v>
       </c>
@@ -6210,7 +6322,7 @@
         <v>i=subsets/a-d/5044/probe</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>67</v>
       </c>
@@ -6245,7 +6357,7 @@
         <v>j=subsets/r--/890/no-probe</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B37" s="13" t="s">
         <v>70</v>
       </c>
@@ -6279,8 +6391,12 @@
         <f t="shared" si="0"/>
         <v>k=subsets/v--/890/no-probe</v>
       </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T37" s="13">
+        <f>15130+3*890</f>
+        <v>17800</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B38" s="13" t="s">
         <v>68</v>
       </c>
@@ -6314,7 +6430,7 @@
         <v>l=subsets/r-d/890/no-probe</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B39" s="51" t="s">
         <v>89</v>
       </c>
@@ -6348,7 +6464,7 @@
         <v>m=subsets/v-d/890/no-probe</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B40" s="51" t="s">
         <v>90</v>
       </c>
@@ -6383,7 +6499,7 @@
         <v>n=subsets/a-d/890/no-probe</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B41" s="51" t="s">
         <v>91</v>
       </c>
@@ -6418,7 +6534,7 @@
         <v>o=subsets/v--/594/no-probe</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
         <v>56</v>
       </c>
@@ -6453,7 +6569,7 @@
         <v>p=subsets/r--/445/no-probe</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B43" s="13" t="s">
         <v>71</v>
       </c>
@@ -6488,7 +6604,7 @@
         <v>q=subsets/v--/445/no-probe</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B44" s="13" t="s">
         <v>35</v>
       </c>
@@ -6523,7 +6639,7 @@
         <v>r=subsets/r-d/445/no-probe</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B45" s="51" t="s">
         <v>92</v>
       </c>
@@ -6558,7 +6674,7 @@
         <v>s=subsets/v-d/445/no-probe</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B46" s="13" t="s">
         <v>57</v>
       </c>
@@ -6593,7 +6709,7 @@
         <v>t=subsets/a-d/445/no-probe</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>41</v>
       </c>
@@ -6628,7 +6744,7 @@
         <v>u=subsets/r--/297/no-probe</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B48" s="13" t="s">
         <v>0</v>
       </c>
@@ -6663,7 +6779,7 @@
         <v>v=subsets/r-d/297/no-probe</v>
       </c>
     </row>
-    <row r="49" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G49" s="13" t="s">
         <v>41</v>
       </c>
@@ -6689,7 +6805,7 @@
         <v>w=subsets/v-d/297/no-probe</v>
       </c>
     </row>
-    <row r="50" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G50" s="13" t="s">
         <v>0</v>
       </c>
@@ -6715,7 +6831,7 @@
         <v>x=subsets/a-d/297/no-probe</v>
       </c>
     </row>
-    <row r="51" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G51" s="51" t="s">
         <v>126</v>
       </c>
@@ -6741,7 +6857,7 @@
         <v>j_p=subsets/r--/890/probe</v>
       </c>
     </row>
-    <row r="52" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G52" s="51" t="s">
         <v>127</v>
       </c>
@@ -6767,7 +6883,7 @@
         <v>k_p=subsets/v--/890/probe</v>
       </c>
     </row>
-    <row r="53" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G53" s="51" t="s">
         <v>128</v>
       </c>
@@ -6793,7 +6909,7 @@
         <v>o_p=subsets/v--/594/probe</v>
       </c>
     </row>
-    <row r="54" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G54" s="51" t="s">
         <v>129</v>
       </c>
@@ -6819,7 +6935,7 @@
         <v>p_p=subsets/r--/445/probe</v>
       </c>
     </row>
-    <row r="55" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G55" s="51" t="s">
         <v>130</v>
       </c>
@@ -6845,7 +6961,7 @@
         <v>q_p=subsets/v--/445/probe</v>
       </c>
     </row>
-    <row r="56" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G56" s="51" t="s">
         <v>131</v>
       </c>
@@ -6897,59 +7013,59 @@
       <selection activeCell="R27" sqref="R27:S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>119658</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>15405</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>136476</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>119442</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>119889</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>130050</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>128383</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>121819</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>SUM(A1:A8)</f>
         <v>891122</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -6987,7 +7103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -7025,7 +7141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -7063,7 +7179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -7101,7 +7217,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -7139,7 +7255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -7177,7 +7293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2023</v>
       </c>
@@ -7215,7 +7331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2023</v>
       </c>
@@ -7253,7 +7369,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="57">
         <f>DATE(A14,B14,C14)</f>
         <v>45265</v>
@@ -7311,7 +7427,7 @@
         <v>57640</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="57">
         <f t="shared" ref="A24:A30" si="0">DATE(A15,B15,C15)</f>
         <v>45265</v>
@@ -7337,7 +7453,7 @@
         <v>0.80287037037037035</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="57">
         <f t="shared" si="0"/>
         <v>45266</v>
@@ -7363,7 +7479,7 @@
         <v>0.8410185185185185</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="57">
         <f t="shared" si="0"/>
         <v>45268</v>
@@ -7404,7 +7520,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="57">
         <f t="shared" si="0"/>
         <v>45268</v>
@@ -7434,7 +7550,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="57">
         <f t="shared" si="0"/>
         <v>45272</v>
@@ -7464,7 +7580,7 @@
         <v>1.6166666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="57">
         <f t="shared" si="0"/>
         <v>45272</v>
@@ -7490,7 +7606,7 @@
         <v>0.86751157407407409</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="57">
         <f t="shared" si="0"/>
         <v>45273</v>
@@ -7525,16 +7641,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466E9C9-12DD-4ED3-9EAA-071EF16B3A1C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>141</v>
       </c>
@@ -7551,7 +7667,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -7565,7 +7681,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -7576,7 +7692,7 @@
         <v>45358.711796412033</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -7590,7 +7706,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -7601,7 +7717,7 @@
         <v>45361</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -7612,7 +7728,7 @@
         <v>45361.458225925926</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -7623,7 +7739,7 @@
         <v>45358.796980555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -7634,7 +7750,7 @@
         <v>45361</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -7663,9 +7779,9 @@
       <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>156</v>
       </c>
@@ -7673,7 +7789,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7685,7 +7801,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7697,7 +7813,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7709,7 +7825,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7721,7 +7837,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7733,7 +7849,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7745,7 +7861,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7757,7 +7873,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7769,7 +7885,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7781,7 +7897,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7793,7 +7909,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7805,7 +7921,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7817,7 +7933,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7829,7 +7945,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7841,7 +7957,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -7853,7 +7969,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -7865,7 +7981,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -7877,7 +7993,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -7889,7 +8005,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -7901,7 +8017,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -7913,7 +8029,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -7925,7 +8041,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -7937,7 +8053,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -7949,7 +8065,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -7961,7 +8077,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -7973,7 +8089,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -7985,7 +8101,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -7997,7 +8113,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -8009,7 +8125,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -8021,7 +8137,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -8033,7 +8149,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -8045,7 +8161,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -8057,7 +8173,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -8069,7 +8185,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -8081,7 +8197,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -8093,7 +8209,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -8105,7 +8221,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -8117,7 +8233,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -8129,7 +8245,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -8141,7 +8257,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -8153,7 +8269,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -8165,7 +8281,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -8177,7 +8293,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -8189,7 +8305,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -8201,7 +8317,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -8213,7 +8329,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -8225,7 +8341,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -8237,7 +8353,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -8249,7 +8365,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -8261,7 +8377,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -8273,7 +8389,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -8285,7 +8401,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -8297,7 +8413,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -8309,7 +8425,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -8321,7 +8437,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -8333,7 +8449,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -8345,7 +8461,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -8357,7 +8473,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -8369,7 +8485,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -8381,7 +8497,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -8393,7 +8509,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -8405,7 +8521,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -8417,7 +8533,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -8429,7 +8545,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -8441,7 +8557,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -8460,6 +8576,187 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A4B4B6-2EEA-7E41-95D7-7FFF86355933}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159ABB3B-8086-4C4F-9625-D0E2E1276B9A}">
   <dimension ref="B2:H26"/>
   <sheetViews>
@@ -8467,14 +8764,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="8" width="9.140625" style="2"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="2"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
@@ -8491,7 +8788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8512,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -8530,7 +8827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -8548,7 +8845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
@@ -8567,7 +8864,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>2</v>
       </c>
@@ -8584,7 +8881,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
@@ -8601,7 +8898,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>1</v>
       </c>
@@ -8618,7 +8915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
@@ -8635,7 +8932,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
@@ -8652,7 +8949,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>3</v>
       </c>
@@ -8669,7 +8966,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -8683,7 +8980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="4">
         <v>0</v>
       </c>
@@ -8697,7 +8994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <v>1</v>
       </c>
@@ -8711,7 +9008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="4">
         <v>2</v>
       </c>
@@ -8725,7 +9022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <v>3</v>
       </c>
@@ -8744,7 +9041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122C5CE7-0A9B-40E5-82A0-8A91F53708D4}">
   <dimension ref="A1:S27"/>
   <sheetViews>
@@ -8752,21 +9049,21 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="16" max="16" width="2.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.1640625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" customWidth="1"/>
+    <col min="16" max="16" width="2.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5" style="15" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -8796,7 +9093,7 @@
         <v>22437.777777777777</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>22</v>
       </c>
@@ -8838,7 +9135,7 @@
         <v>19072.111111111109</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -8878,7 +9175,7 @@
         <v>1121.8888888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>101564</v>
       </c>
@@ -8912,7 +9209,7 @@
         <v>1121.8888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F5" s="16" t="s">
         <v>27</v>
       </c>
@@ -8939,7 +9236,7 @@
         <v>1121.8888888888889</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -8950,7 +9247,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
@@ -8970,7 +9267,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -8986,7 +9283,7 @@
         <v>0.94092871433084135</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>39177</v>
       </c>
@@ -8998,7 +9295,7 @@
         <v>4926</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>88624</v>
       </c>
@@ -9013,7 +9310,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>90391</v>
       </c>
@@ -9026,7 +9323,7 @@
       </c>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>99090</v>
       </c>
@@ -9039,7 +9336,7 @@
       </c>
       <c r="D12" s="16"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>55</v>
       </c>
@@ -9066,7 +9363,7 @@
         <v>23420</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>48</v>
       </c>
@@ -9109,7 +9406,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="17" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>3</v>
       </c>
@@ -9153,7 +9450,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="18" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>34</v>
       </c>
@@ -9197,7 +9494,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="19" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F19">
         <f>SUM(F16:F18)</f>
         <v>20194</v>
@@ -9239,7 +9536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F20">
         <f>F19/1172</f>
         <v>17.230375426621162</v>
@@ -9267,7 +9564,7 @@
       </c>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:19" x14ac:dyDescent="0.2">
       <c r="I21" s="19" t="s">
         <v>47</v>
       </c>
@@ -9291,7 +9588,7 @@
       </c>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:19" x14ac:dyDescent="0.2">
       <c r="I22" s="19" t="s">
         <v>47</v>
       </c>
@@ -9314,7 +9611,7 @@
         <v>0.38061324576741012</v>
       </c>
     </row>
-    <row r="23" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:19" x14ac:dyDescent="0.2">
       <c r="I23" s="19" t="s">
         <v>47</v>
       </c>
@@ -9337,7 +9634,7 @@
         <v>8.7722290929250712E-2</v>
       </c>
     </row>
-    <row r="26" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:19" x14ac:dyDescent="0.2">
       <c r="M26">
         <f>SUM(M16:M23)</f>
         <v>23449</v>
@@ -9350,7 +9647,7 @@
         <v>18756</v>
       </c>
     </row>
-    <row r="27" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:19" x14ac:dyDescent="0.2">
       <c r="N27">
         <f>M26-N26</f>
         <v>4689.7999999999993</v>
@@ -9399,17 +9696,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE7D156-8A4C-4FD8-B490-BA9051D7D7C4}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -9426,7 +9723,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9443,7 +9740,7 @@
         <v>1.5868009999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9460,7 +9757,7 @@
         <v>1.5954137E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -9477,7 +9774,7 @@
         <v>7.8926929999999992E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -9494,7 +9791,7 @@
         <v>1.5835911000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -9511,7 +9808,7 @@
         <v>2.0469496E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -9528,7 +9825,7 @@
         <v>3.7692994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -9545,7 +9842,7 @@
         <v>4.9928285000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -9562,7 +9859,7 @@
         <v>4.2487080000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -9579,7 +9876,7 @@
         <v>7.3230886000000004E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -9596,7 +9893,7 @@
         <v>7.4917830000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -9613,7 +9910,7 @@
         <v>6.5534750000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -9624,7 +9921,7 @@
         <v>5.8172493999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9635,7 +9932,7 @@
         <v>4.8101579999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9646,7 +9943,7 @@
         <v>3.6676704999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9657,7 +9954,7 @@
         <v>0.11926489999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -9668,7 +9965,7 @@
         <v>2.1976442999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -9679,7 +9976,7 @@
         <v>1.3617169E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -9690,7 +9987,7 @@
         <v>1.3073108999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -9701,7 +9998,7 @@
         <v>2.2888578E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -9712,7 +10009,7 @@
         <v>2.3160355000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -9723,7 +10020,7 @@
         <v>3.7845414000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -9734,7 +10031,7 @@
         <v>0.12233808</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -9745,7 +10042,7 @@
         <v>1.5967700000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -9756,7 +10053,7 @@
         <v>8.572161E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -9767,7 +10064,7 @@
         <v>1.2902888499999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -9778,7 +10075,7 @@
         <v>2.1054586E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -9789,7 +10086,7 @@
         <v>1.4843863000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -9800,7 +10097,7 @@
         <v>1.6115543E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -9811,7 +10108,7 @@
         <v>1.6760988000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -9822,7 +10119,7 @@
         <v>1.6937934000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -9833,7 +10130,7 @@
         <v>3.1489110000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -9844,7 +10141,7 @@
         <v>2.0184044000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -9855,7 +10152,7 @@
         <v>2.8597627E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -9866,7 +10163,7 @@
         <v>0.10342193</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -9877,7 +10174,7 @@
         <v>7.9037419999999997E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -9888,7 +10185,7 @@
         <v>3.7345152E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -9899,7 +10196,7 @@
         <v>2.9099640999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -9910,7 +10207,7 @@
         <v>1.6656154999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -9921,7 +10218,7 @@
         <v>2.2970185000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -9932,7 +10229,7 @@
         <v>4.3361972999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42">
         <f>B43/1000</f>
         <v>0.66200000000000003</v>
@@ -9942,7 +10239,7 @@
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>662</v>
       </c>
@@ -9965,15 +10262,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>15</xdr:col>
-                    <xdr:colOff>447675</xdr:colOff>
+                    <xdr:colOff>444500</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9987,15 +10284,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:colOff>254000</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>50800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:colOff>546100</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:rowOff>88900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>